<commit_message>
Fixed Excel Download Format, Added SSL Certificates for webserver  (GreenLock Module)
</commit_message>
<xml_diff>
--- a/Report Pack/excel_modules/report_pack_templ.xlsx
+++ b/Report Pack/excel_modules/report_pack_templ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vakishnathayalan/Dev/projectb/Report Pack/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61468\Dev\tesproj\projectb\Report Pack\excel_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA2D02B-0EA7-DE44-907F-416CF11825FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AEA512-7609-4A88-9020-43ADB92951C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="15940" windowWidth="22760" windowHeight="18480" xr2:uid="{1380735C-F8DC-1F43-8BDF-2AE10963A1DD}"/>
+    <workbookView xWindow="1140" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{1380735C-F8DC-1F43-8BDF-2AE10963A1DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Card Payments</t>
   </si>
@@ -58,59 +58,38 @@
     <t>Dishonored Direct Debits</t>
   </si>
   <si>
-    <t>Number of Active Authorities</t>
-  </si>
-  <si>
-    <t>Fee Finance</t>
-  </si>
-  <si>
-    <t>Fee Finance Loans</t>
-  </si>
-  <si>
-    <t>Fee Finance Quotes</t>
-  </si>
-  <si>
-    <t>Engagements</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Engagements Sent</t>
-  </si>
-  <si>
-    <t>Engagements by Status</t>
-  </si>
-  <si>
-    <t>Engagements Signed</t>
-  </si>
-  <si>
     <t>Debtor Management</t>
   </si>
   <si>
-    <t>Aged Debt Trend</t>
-  </si>
-  <si>
     <t>Number of Reminders Sent</t>
   </si>
   <si>
-    <t>Credit Insights</t>
-  </si>
-  <si>
-    <t>Credit Scores Descriptor</t>
-  </si>
-  <si>
-    <t>Clients Dropped Credit Status</t>
-  </si>
-  <si>
-    <t>Credit Scores by State</t>
+    <t>Count of Clients Dropped Credit Scores</t>
+  </si>
+  <si>
+    <t>Credit Score Descriptor Trend</t>
+  </si>
+  <si>
+    <t>Fair</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>No Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +113,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -176,6 +163,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,7 +195,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1179210</xdr:colOff>
+      <xdr:colOff>902985</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
@@ -559,16 +550,16 @@
   <dimension ref="A5:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="B14:C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.75" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="19.5" thickBot="1">
       <c r="B5" s="2">
         <v>44197</v>
       </c>
@@ -591,7 +582,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="22" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="21" thickTop="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +594,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -615,7 +606,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -627,7 +618,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -639,7 +630,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="20.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -651,7 +642,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18.75">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -663,7 +654,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18.75">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -675,7 +666,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -687,9 +678,9 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
+    <row r="14" spans="1:8" ht="20.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -699,9 +690,9 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
+    <row r="15" spans="1:8" ht="18.75">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -711,9 +702,9 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -723,9 +714,9 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>10</v>
+    <row r="17" spans="1:8" ht="18.75">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -735,9 +726,9 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
+    <row r="18" spans="1:8" ht="18.75">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -747,12 +738,12 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
+    <row r="19" spans="1:8" ht="18.75">
+      <c r="A19" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -761,8 +752,8 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:8" ht="18.75">
+      <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="4"/>
@@ -773,8 +764,8 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:8" ht="18.75">
+      <c r="A21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="4"/>
@@ -785,10 +776,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="22" spans="1:8" ht="18.75">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -797,10 +785,8 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="23" spans="1:8" ht="18.75">
+      <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -809,10 +795,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="24" spans="1:8" ht="18.75">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -821,10 +804,8 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="25" spans="1:8" ht="20.25">
+      <c r="A25" s="1"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -833,10 +814,8 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>20</v>
-      </c>
+    <row r="26" spans="1:8" ht="18.75">
+      <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -845,10 +824,8 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>21</v>
-      </c>
+    <row r="27" spans="1:8" ht="18.75">
+      <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -857,10 +834,8 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>22</v>
-      </c>
+    <row r="28" spans="1:8" ht="18.75">
+      <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -871,6 +846,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>